<commit_message>
FMP API was made non-free.  Temporarily switched to tiingo for data_mod
</commit_message>
<xml_diff>
--- a/outputs/outperformance.xlsx
+++ b/outputs/outperformance.xlsx
@@ -456,37 +456,37 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1675054846835838</v>
+        <v>-0.1014498015221799</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1636683359043037</v>
+        <v>-0.004298632242113798</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1266782114757333</v>
+        <v>-0.1764483179748445</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.1677436996032099</v>
+        <v>-0.03704488548387895</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7145499389330037</v>
+        <v>0.5424933017368545</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2078061248566231</v>
+        <v>-0.3483997890283307</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.3840263231347335</v>
+        <v>0.02882171812868239</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.3311871597487191</v>
+        <v>0.3724078955536167</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2479111539892746</v>
+        <v>-0.06198631201144565</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1582001925184242</v>
+        <v>-1.95748049505588</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2992287713242997</v>
+        <v>0.3398290965197098</v>
       </c>
     </row>
     <row r="3">
@@ -497,37 +497,37 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1437247512895216</v>
+        <v>-0.3251547915878432</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.361254657775409</v>
+        <v>0.1481789530726816</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.478696484693499</v>
+        <v>-0.1280136405857694</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.8220499208640279</v>
+        <v>0.1239553757617533</v>
       </c>
       <c r="G3" t="n">
-        <v>1.534956674404611</v>
+        <v>0.8941861805673083</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.9507665601252733</v>
+        <v>0.03814114661730883</v>
       </c>
       <c r="I3" t="n">
-        <v>-3.166532145484353</v>
+        <v>-0.4251959275780741</v>
       </c>
       <c r="J3" t="n">
-        <v>-2.16438436199622</v>
+        <v>0.8773647496340542</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7035593791441748</v>
+        <v>-0.084303640647092</v>
       </c>
       <c r="L3" t="n">
-        <v>1.980929043869383</v>
+        <v>-3.808591867838291</v>
       </c>
       <c r="M3" t="n">
-        <v>-3.651436379671482</v>
+        <v>1.118471141366099</v>
       </c>
     </row>
     <row r="4">
@@ -538,37 +538,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.1534695453779622</v>
+        <v>-0.7909427573011025</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2450302276637982</v>
+        <v>-0.09200447355101615</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.8592916986689687</v>
+        <v>-0.7072248548488091</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.5006298994977267</v>
+        <v>-0.04204534001296334</v>
       </c>
       <c r="G4" t="n">
-        <v>2.007852759087354</v>
+        <v>2.377435877601563</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.60290434158239</v>
+        <v>-0.2360825738701717</v>
       </c>
       <c r="I4" t="n">
-        <v>-2.789936510070966</v>
+        <v>-3.068242518174258</v>
       </c>
       <c r="J4" t="n">
-        <v>-1.705730395511779</v>
+        <v>-0.1306452463718342</v>
       </c>
       <c r="K4" t="n">
-        <v>0.524264048285225</v>
+        <v>-0.1611525627603123</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5071487596148011</v>
+        <v>-3.816099869890487</v>
       </c>
       <c r="M4" t="n">
-        <v>-3.157498132590928</v>
+        <v>-1.130861331586144</v>
       </c>
     </row>
     <row r="5">
@@ -579,37 +579,37 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.5230028957495195</v>
+        <v>-0.619462737100814</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2278418749125907</v>
+        <v>0.3123223774254897</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.8412514497987902</v>
+        <v>-0.3161459340758013</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.01715574604858228</v>
+        <v>0.1168638119744382</v>
       </c>
       <c r="G5" t="n">
-        <v>1.023666243618585</v>
+        <v>1.165558098105889</v>
       </c>
       <c r="H5" t="n">
-        <v>-1.232136516001631</v>
+        <v>-1.133427336932098</v>
       </c>
       <c r="I5" t="n">
-        <v>-2.006634433271381</v>
+        <v>-2.787272713319324</v>
       </c>
       <c r="J5" t="n">
-        <v>-1.098100111220224</v>
+        <v>-0.1251017220096353</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5097710947928329</v>
+        <v>-0.06128557859166428</v>
       </c>
       <c r="L5" t="n">
-        <v>-2.45594925337131</v>
+        <v>-5.406609340606341</v>
       </c>
       <c r="M5" t="n">
-        <v>-4.036084926957502</v>
+        <v>-0.06307990344230563</v>
       </c>
     </row>
     <row r="6">
@@ -620,37 +620,37 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-1.101297853974287</v>
+        <v>-2.015829499669683</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3498554937523979</v>
+        <v>-0.7949578559213135</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.568612000532794</v>
+        <v>-1.394434082777019</v>
       </c>
       <c r="F6" t="n">
-        <v>1.13201196674111</v>
+        <v>1.334930734256413</v>
       </c>
       <c r="G6" t="n">
-        <v>1.560906043821927</v>
+        <v>-1.57175418577667</v>
       </c>
       <c r="H6" t="n">
-        <v>-2.355300536817427</v>
+        <v>-1.996265866123863</v>
       </c>
       <c r="I6" t="n">
-        <v>-6.399917156514263</v>
+        <v>-5.834707070587831</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.023536691344824</v>
+        <v>0.2345879399825267</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.1058341627669495</v>
+        <v>-0.7400711181697074</v>
       </c>
       <c r="L6" t="n">
-        <v>-7.607592798349829</v>
+        <v>-9.29325863300001</v>
       </c>
       <c r="M6" t="n">
-        <v>-4.807630835253553</v>
+        <v>-2.614532489909299</v>
       </c>
     </row>
     <row r="7">
@@ -661,37 +661,37 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.2245316479516867</v>
+        <v>-0.3848169996572235</v>
       </c>
       <c r="D7" t="n">
-        <v>0.07350766708508816</v>
+        <v>-0.1069831284718319</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.3745923383398461</v>
+        <v>-0.3072903339198688</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2218767906594914</v>
+        <v>0.2342638477219571</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2964365981291643</v>
+        <v>-0.322204328610485</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.4362555312640236</v>
+        <v>-0.3409918856266996</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.903850298772025</v>
+        <v>-1.247764610678042</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.2157951365854688</v>
+        <v>0.04999113158700405</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.0202325194904862</v>
+        <v>-0.1289650951224796</v>
       </c>
       <c r="L7" t="n">
-        <v>-1.325611189801717</v>
+        <v>-1.473840504439615</v>
       </c>
       <c r="M7" t="n">
-        <v>-1.133084347808176</v>
+        <v>-0.5386458857125009</v>
       </c>
     </row>
     <row r="8">
@@ -706,34 +706,34 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.02649242028227954</v>
+        <v>0.03523207401696232</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1209499480429519</v>
+        <v>0.1707156334231804</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4040288969158111</v>
+        <v>-0.04897352782279507</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1987088444157538</v>
+        <v>0.07293463143254549</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.03961995249406126</v>
+        <v>0.03462434712735993</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.08627763393746271</v>
+        <v>-0.02637449449825977</v>
       </c>
       <c r="I8" t="n">
-        <v>0.01044399596367318</v>
+        <v>-0.03540280097648716</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.2076920270023726</v>
+        <v>-0.01690357023690286</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.7179287471916159</v>
+        <v>-1.205272360457297</v>
       </c>
       <c r="M8" t="n">
         <v>-0</v>
@@ -747,34 +747,34 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>-0.1083115525352854</v>
+        <v>0.08030840400925246</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.2765301350883262</v>
+        <v>0.307181940700808</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.911169769380381</v>
+        <v>-0.3038357644516427</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.8021949644932261</v>
+        <v>0.09449791376912296</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.6682565320665065</v>
+        <v>0.04635194857372462</v>
       </c>
       <c r="H9" t="n">
-        <v>0.07969328818960389</v>
+        <v>-0.1256540957396791</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1947998654557692</v>
+        <v>-0.05372478478735724</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.8470790001824506</v>
+        <v>0.1198164831498179</v>
       </c>
       <c r="K9" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9464619664063345</v>
+        <v>-1.928786146603902</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -788,34 +788,34 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.08181913225300527</v>
+        <v>0.02422205088666231</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1695687564946291</v>
+        <v>0.3050579514824803</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.472492358988605</v>
+        <v>-2.300756347920036</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.5659522272433885</v>
+        <v>-0.172506258692635</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.6425035629453649</v>
+        <v>-0.3289312977099215</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0326946823341951</v>
+        <v>-0.09584877268880089</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1702758156744034</v>
+        <v>0.02151355518437605</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.5333661740558309</v>
+        <v>-0.2326726726726727</v>
       </c>
       <c r="K10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.2006633144324393</v>
+        <v>-2.390398453261602</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -829,34 +829,34 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.008050182958703798</v>
+        <v>0.05815882806476527</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.02251818496709555</v>
+        <v>0.4083369272237197</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.920727979994439</v>
+        <v>-1.916963803349533</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.4202324080051683</v>
+        <v>-0.1896300417246252</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.3968598574821814</v>
+        <v>-0.08153475291281358</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.2676877116112307</v>
+        <v>-0.3568061694723975</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1253279515640771</v>
+        <v>-0.02464602338429955</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.1995365809158869</v>
+        <v>-0.1118618618618612</v>
       </c>
       <c r="K11" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>-1.948663742377218</v>
+        <v>-3.566765299260248</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -870,34 +870,34 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1492943021432301</v>
+        <v>0.2287494217424826</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6937989262209892</v>
+        <v>0.9769022911051198</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.604084467907763</v>
+        <v>-2.428687196110217</v>
       </c>
       <c r="F12" t="n">
-        <v>0.05666881859265176</v>
+        <v>0.3640389429763641</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1736674584323073</v>
+        <v>0.1239775010044249</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.7610595498904633</v>
+        <v>-0.8454848114360983</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.07488731920618831</v>
+        <v>-0.1657844019015801</v>
       </c>
       <c r="J12" t="n">
-        <v>0.6540667761357358</v>
+        <v>0.8531331331331271</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>-6.014325452016682</v>
+        <v>-6.958345662407524</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -911,34 +911,34 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.03024546511133203</v>
+        <v>0.04230667805838186</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1328111067063249</v>
+        <v>0.1687007801919856</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.8559365135805147</v>
+        <v>-0.7246048173976746</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0121360063209671</v>
+        <v>0.06995941223218735</v>
       </c>
       <c r="G13" t="n">
-        <v>0.03583958306310669</v>
+        <v>0.02444171289232733</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1465170827534296</v>
+        <v>-0.1515469261466029</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.01524987270580663</v>
+        <v>-0.02981171403260093</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1306448589584163</v>
+        <v>0.1570672701527503</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>-1.078909410318606</v>
+        <v>-1.146178428443042</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -956,37 +956,37 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.1939979049658634</v>
+        <v>-0.1366818755391422</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.2846182839472556</v>
+        <v>-0.1750142656652942</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.2773506854400778</v>
+        <v>-0.1274747901520494</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03096514481254395</v>
+        <v>-0.1099795169164244</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7541698914270649</v>
+        <v>0.5078689546094945</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2940837587940858</v>
+        <v>-0.3220252945300709</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.3944703190984067</v>
+        <v>0.06422451910516955</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.1234951327463465</v>
+        <v>0.3893114657905196</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2479111539892746</v>
+        <v>-0.06198631201144565</v>
       </c>
       <c r="L14" t="n">
-        <v>0.8761289397100401</v>
+        <v>-0.7522081345985829</v>
       </c>
       <c r="M14" t="n">
-        <v>0.2992287713242997</v>
+        <v>0.3398290965197098</v>
       </c>
     </row>
     <row r="15">
@@ -997,37 +997,37 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.2520363038248069</v>
+        <v>-0.4054631955970956</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.0847245226870828</v>
+        <v>-0.1590029876281264</v>
       </c>
       <c r="E15" t="n">
-        <v>0.4324732846868822</v>
+        <v>0.1758221238658733</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.01985495637080181</v>
+        <v>0.02945746199263036</v>
       </c>
       <c r="G15" t="n">
-        <v>2.203213206471117</v>
+        <v>0.8478342319935837</v>
       </c>
       <c r="H15" t="n">
-        <v>-1.030459848314877</v>
+        <v>0.1637952423569879</v>
       </c>
       <c r="I15" t="n">
-        <v>-3.361332010940123</v>
+        <v>-0.3714711427907169</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.317305361813769</v>
+        <v>0.7575482664842363</v>
       </c>
       <c r="K15" t="n">
-        <v>0.7035593791441748</v>
+        <v>-0.084303640647092</v>
       </c>
       <c r="L15" t="n">
-        <v>1.034467077463048</v>
+        <v>-1.879805721234389</v>
       </c>
       <c r="M15" t="n">
-        <v>-3.651436379671482</v>
+        <v>1.118471141366099</v>
       </c>
     </row>
     <row r="16">
@@ -1038,37 +1038,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.07165041312495693</v>
+        <v>-0.8151648081877648</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.0754614711691691</v>
+        <v>-0.3970624250334965</v>
       </c>
       <c r="E16" t="n">
-        <v>1.613200660319637</v>
+        <v>1.593531493071227</v>
       </c>
       <c r="F16" t="n">
-        <v>0.06532232774566171</v>
+        <v>0.1304609186796717</v>
       </c>
       <c r="G16" t="n">
-        <v>2.65035632203272</v>
+        <v>2.706367175311484</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.6355990239165852</v>
+        <v>-0.1402338011813708</v>
       </c>
       <c r="I16" t="n">
-        <v>-2.96021232574537</v>
+        <v>-3.089756073358634</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.172364221455948</v>
+        <v>0.1020274263008385</v>
       </c>
       <c r="K16" t="n">
-        <v>0.524264048285225</v>
+        <v>-0.1611525627603123</v>
       </c>
       <c r="L16" t="n">
-        <v>0.7078120740472403</v>
+        <v>-1.425701416628885</v>
       </c>
       <c r="M16" t="n">
-        <v>-3.157498132590928</v>
+        <v>-1.130861331586144</v>
       </c>
     </row>
     <row r="17">
@@ -1079,37 +1079,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.5149527127908158</v>
+        <v>-0.6776215651655793</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2503600598796862</v>
+        <v>-0.09601454979822999</v>
       </c>
       <c r="E17" t="n">
-        <v>2.079476530195649</v>
+        <v>1.600817869273732</v>
       </c>
       <c r="F17" t="n">
-        <v>0.403076661956586</v>
+        <v>0.3064938536990633</v>
       </c>
       <c r="G17" t="n">
-        <v>1.420526101100767</v>
+        <v>1.247092851018703</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.9644488043904007</v>
+        <v>-0.7766211674597</v>
       </c>
       <c r="I17" t="n">
-        <v>-2.131962384835458</v>
+        <v>-2.762626689935024</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.8985635303043373</v>
+        <v>-0.0132398601477741</v>
       </c>
       <c r="K17" t="n">
-        <v>0.5097710947928329</v>
+        <v>-0.06128557859166428</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.5072855109940919</v>
+        <v>-1.839844041346093</v>
       </c>
       <c r="M17" t="n">
-        <v>-4.036084926957502</v>
+        <v>-0.06307990344230563</v>
       </c>
     </row>
     <row r="18">
@@ -1120,37 +1120,37 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-1.250592156117517</v>
+        <v>-2.244578921412165</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.3439434324685913</v>
+        <v>-1.771860147026433</v>
       </c>
       <c r="E18" t="n">
-        <v>1.035472467374969</v>
+        <v>1.034253113333197</v>
       </c>
       <c r="F18" t="n">
-        <v>1.075343148148458</v>
+        <v>0.9708917912800484</v>
       </c>
       <c r="G18" t="n">
-        <v>1.38723858538962</v>
+        <v>-1.695731686781095</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.594240986926963</v>
+        <v>-1.150781054687765</v>
       </c>
       <c r="I18" t="n">
-        <v>-6.325029837308075</v>
+        <v>-5.668922668686251</v>
       </c>
       <c r="J18" t="n">
-        <v>-1.67760346748056</v>
+        <v>-0.6185451931506004</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.1058341627669495</v>
+        <v>-0.7400711181697074</v>
       </c>
       <c r="L18" t="n">
-        <v>-1.593267346333147</v>
+        <v>-2.334912970592486</v>
       </c>
       <c r="M18" t="n">
-        <v>-4.807630835253553</v>
+        <v>-2.614532489909299</v>
       </c>
     </row>
     <row r="19">
@@ -1161,37 +1161,37 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.2547771130630188</v>
+        <v>-0.4271236777156054</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.05930343962123671</v>
+        <v>-0.2756839086638175</v>
       </c>
       <c r="E19" t="n">
-        <v>0.4813441752406686</v>
+        <v>0.4173144834778058</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2097407843385243</v>
+        <v>0.1643044354897697</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2605970150660576</v>
+        <v>-0.3466460415028123</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.289738448510594</v>
+        <v>-0.1894449594800967</v>
       </c>
       <c r="I19" t="n">
-        <v>-1.888600426066218</v>
+        <v>-1.217952896645441</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.3464399955438851</v>
+        <v>-0.1070761385657463</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.0202325194904862</v>
+        <v>-0.1289650951224796</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.2467017794831114</v>
+        <v>-0.3276620759965734</v>
       </c>
       <c r="M19" t="n">
-        <v>-1.133084347808176</v>
+        <v>-0.5386458857125009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated some trades and adjusted closing prices
</commit_message>
<xml_diff>
--- a/outputs/outperformance.xlsx
+++ b/outputs/outperformance.xlsx
@@ -379,7 +379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,11 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Fixed Income</t>
         </is>
       </c>
@@ -456,37 +461,40 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.1014498015221799</v>
+        <v>-0.1489810950416438</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.004298632242113798</v>
+        <v>-0.2043474562481407</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.1764483179748445</v>
+        <v>-0.2547938095604285</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.03704488548387895</v>
+        <v>-0.0283171465889092</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5424933017368545</v>
+        <v>-1.561687929733194</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.3483997890283307</v>
+        <v>0.2521240374853275</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02882171812868239</v>
+        <v>-0.07928124633826795</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3724078955536167</v>
+        <v>0.02041826591931516</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.06198631201144565</v>
+        <v>0.02378011117973977</v>
       </c>
       <c r="L2" t="n">
-        <v>-1.95748049505588</v>
+        <v>-0.2098342518997854</v>
       </c>
       <c r="M2" t="n">
-        <v>0.3398290965197098</v>
+        <v>-0.5453174658749476</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.260637167218768</v>
       </c>
     </row>
     <row r="3">
@@ -497,37 +505,40 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.3251547915878432</v>
+        <v>-0.4062303152217909</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1481789530726816</v>
+        <v>-0.03086517683768375</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.1280136405857694</v>
+        <v>-0.2300319671529607</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1239553757617533</v>
+        <v>-0.03032195891464575</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8941861805673083</v>
+        <v>-1.186312698696654</v>
       </c>
       <c r="H3" t="n">
-        <v>0.03814114661730883</v>
+        <v>0.3629622412102476</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.4251959275780741</v>
+        <v>-0.5040763229969668</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8773647496340542</v>
+        <v>0.6147778012059749</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.084303640647092</v>
+        <v>-0.2386391904336048</v>
       </c>
       <c r="L3" t="n">
-        <v>-3.808591867838291</v>
+        <v>-2.109982518704936</v>
       </c>
       <c r="M3" t="n">
-        <v>1.118471141366099</v>
+        <v>0.3768739117126277</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.8037272180612992</v>
       </c>
     </row>
     <row r="4">
@@ -538,37 +549,40 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.7909427573011025</v>
+        <v>-0.7169975486779477</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.09200447355101615</v>
+        <v>-0.2946698798083034</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.7072248548488091</v>
+        <v>-0.06149789202139089</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.04204534001296334</v>
+        <v>0.01091433704255712</v>
       </c>
       <c r="G4" t="n">
-        <v>2.377435877601563</v>
+        <v>0.306022683792049</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.2360825738701717</v>
+        <v>0.1005380592722608</v>
       </c>
       <c r="I4" t="n">
-        <v>-3.068242518174258</v>
+        <v>-3.047512040033329</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.1306452463718342</v>
+        <v>-0.1497267621519438</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.1611525627603123</v>
+        <v>-0.02892383927239406</v>
       </c>
       <c r="L4" t="n">
-        <v>-3.816099869890487</v>
+        <v>-2.592559864161619</v>
       </c>
       <c r="M4" t="n">
-        <v>-1.130861331586144</v>
+        <v>0.2672110784188562</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-0.7978651073472509</v>
       </c>
     </row>
     <row r="5">
@@ -579,37 +593,40 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.619462737100814</v>
+        <v>-0.5414142807543174</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3123223774254897</v>
+        <v>-0.007461755146021876</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.3161459340758013</v>
+        <v>-0.08557828813120216</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1168638119744382</v>
+        <v>0.274611466321977</v>
       </c>
       <c r="G5" t="n">
-        <v>1.165558098105889</v>
+        <v>-0.7103281350806441</v>
       </c>
       <c r="H5" t="n">
-        <v>-1.133427336932098</v>
+        <v>-0.1362701662175447</v>
       </c>
       <c r="I5" t="n">
-        <v>-2.787272713319324</v>
+        <v>-2.945418105643589</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.1251017220096353</v>
+        <v>-0.08326532583783304</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.06128557859166428</v>
+        <v>-0.2787265467134047</v>
       </c>
       <c r="L5" t="n">
-        <v>-5.406609340606341</v>
+        <v>-4.871307790857954</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.06307990344230563</v>
+        <v>0.7994323085619569</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.604667271479058</v>
       </c>
     </row>
     <row r="6">
@@ -620,37 +637,40 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-2.015829499669683</v>
+        <v>-1.273814175376051</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.7949578559213135</v>
+        <v>0.8625605506452008</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.394434082777019</v>
+        <v>-0.3516343311900239</v>
       </c>
       <c r="F6" t="n">
-        <v>1.334930734256413</v>
+        <v>0.8295064829069797</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.57175418577667</v>
+        <v>0.2646541652774737</v>
       </c>
       <c r="H6" t="n">
-        <v>-1.996265866123863</v>
+        <v>-2.295526176009214</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.834707070587831</v>
+        <v>-5.359240583353815</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2345879399825267</v>
+        <v>-0.01152431248113572</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.7400711181697074</v>
+        <v>-1.349267970439772</v>
       </c>
       <c r="L6" t="n">
-        <v>-9.29325863300001</v>
+        <v>-10.56842778552956</v>
       </c>
       <c r="M6" t="n">
-        <v>-2.614532489909299</v>
+        <v>3.943185013355406</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-1.726398582041249</v>
       </c>
     </row>
     <row r="7">
@@ -661,37 +681,40 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.3848169996572235</v>
+        <v>-0.2142419044454809</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.1069831284718319</v>
+        <v>0.1503728058796788</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.3072903339198688</v>
+        <v>-0.05601791128669487</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2342638477219571</v>
+        <v>0.1404504118786588</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.322204328610485</v>
+        <v>0.04807982169657055</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.3409918856266996</v>
+        <v>-0.3776253217542895</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.247764610678042</v>
+        <v>-1.049080538168349</v>
       </c>
       <c r="J7" t="n">
-        <v>0.04999113158700405</v>
+        <v>0.007488712061596708</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.1289650951224796</v>
+        <v>-0.2382796914939904</v>
       </c>
       <c r="L7" t="n">
-        <v>-1.473840504439615</v>
+        <v>-1.680918564179646</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.5386458857125009</v>
+        <v>0.6853788724589751</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-0.3174670141187252</v>
       </c>
     </row>
     <row r="8">
@@ -706,37 +729,40 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.03523207401696232</v>
+        <v>0.01773549883990645</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1707156334231804</v>
+        <v>0.03344697747655328</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.04897352782279507</v>
+        <v>-0.2902820355610058</v>
       </c>
       <c r="F8" t="n">
-        <v>0.07293463143254549</v>
+        <v>-0.01116174402250351</v>
       </c>
       <c r="G8" t="n">
-        <v>0.03462434712735993</v>
+        <v>-0.01692836908134405</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.02637449449825977</v>
+        <v>0.02704656276890775</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.03540280097648716</v>
+        <v>-0.000989563200618839</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.01690357023690286</v>
+        <v>-0.04871881893772213</v>
       </c>
       <c r="K8" t="n">
+        <v>0.02378011117973977</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.1092988668555154</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-0.007527601204413203</v>
+      </c>
+      <c r="N8" t="n">
         <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-1.205272360457297</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-0</v>
       </c>
     </row>
     <row r="9">
@@ -747,36 +773,39 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.08030840400925246</v>
+        <v>0.1955532435975876</v>
       </c>
       <c r="D9" t="n">
-        <v>0.307181940700808</v>
+        <v>0.2316634406487302</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.3038357644516427</v>
+        <v>-0.4144248808142237</v>
       </c>
       <c r="F9" t="n">
-        <v>0.09449791376912296</v>
+        <v>-0.02733816106486643</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04635194857372462</v>
+        <v>0.01173841904374701</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1256540957396791</v>
+        <v>-0.05855074679567809</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.05372478478735724</v>
+        <v>-0.08736632778662594</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1198164831498179</v>
+        <v>0.002565935620940141</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>-0.2386391904336048</v>
       </c>
       <c r="L9" t="n">
-        <v>-1.928786146603902</v>
+        <v>-1.274290772393061</v>
       </c>
       <c r="M9" t="n">
+        <v>0.6701319963834163</v>
+      </c>
+      <c r="N9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -788,36 +817,39 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.02422205088666231</v>
+        <v>0.09140145510292352</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3050579514824803</v>
+        <v>0.2905202403063736</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.300756347920036</v>
+        <v>-1.317140112042914</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.172506258692635</v>
+        <v>-0.09078809605400978</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.3289312977099215</v>
+        <v>-0.2017371767166316</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.09584877268880089</v>
+        <v>-0.04500878434542416</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02151355518437605</v>
+        <v>0.03521847168395729</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.2326726726726727</v>
+        <v>-0.150905054872121</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>-0.02892383927239406</v>
       </c>
       <c r="L10" t="n">
-        <v>-2.390398453261602</v>
+        <v>-2.615659896719902</v>
       </c>
       <c r="M10" t="n">
+        <v>0.9646051872465706</v>
+      </c>
+      <c r="N10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -829,36 +861,39 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.05815882806476527</v>
+        <v>0.1909877564979118</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4083369272237197</v>
+        <v>0.3282389310722448</v>
       </c>
       <c r="E11" t="n">
-        <v>-1.916963803349533</v>
+        <v>-1.224729385953708</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.1896300417246252</v>
+        <v>-0.06429085245209593</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.08153475291281358</v>
+        <v>-0.1102521148231073</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.3568061694723975</v>
+        <v>-0.186738143213691</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.02464602338429955</v>
+        <v>-0.0005636085943564948</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.1118618618618612</v>
+        <v>-0.06378229257892326</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>-0.2787265467134047</v>
       </c>
       <c r="L11" t="n">
-        <v>-3.566765299260248</v>
+        <v>-3.915233991133615</v>
       </c>
       <c r="M11" t="n">
+        <v>1.349852520276009</v>
+      </c>
+      <c r="N11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -870,36 +905,39 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.2287494217424826</v>
+        <v>0.8386172526222808</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9769022911051198</v>
+        <v>1.027109951478823</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.428687196110217</v>
+        <v>-0.9211664984126267</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3640389429763641</v>
+        <v>0.3607554133549377</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1239775010044249</v>
+        <v>0.2875776170783487</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.8454848114360983</v>
+        <v>-0.5264940492721689</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.1657844019015801</v>
+        <v>-0.4025158197733269</v>
       </c>
       <c r="J12" t="n">
-        <v>0.8531331331331271</v>
+        <v>0.754839523181165</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>-1.349267970439772</v>
       </c>
       <c r="L12" t="n">
-        <v>-6.958345662407524</v>
+        <v>-9.061371058999205</v>
       </c>
       <c r="M12" t="n">
+        <v>1.624013827346932</v>
+      </c>
+      <c r="N12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -911,36 +949,39 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.04230667805838186</v>
+        <v>0.1493464753321933</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1687007801919856</v>
+        <v>0.1742557189694822</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.7246048173976746</v>
+        <v>-0.2479797273564791</v>
       </c>
       <c r="F13" t="n">
-        <v>0.06995941223218735</v>
+        <v>0.06583425231915273</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02444171289232733</v>
+        <v>0.05178587098626595</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1515469261466029</v>
+        <v>-0.0922504335250682</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.02981171403260093</v>
+        <v>-0.07035826605024999</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1570672701527503</v>
+        <v>0.1334791526336825</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>-0.2382796914939904</v>
       </c>
       <c r="L13" t="n">
-        <v>-1.146178428443042</v>
+        <v>-1.47405577885728</v>
       </c>
       <c r="M13" t="n">
+        <v>0.3066904066269789</v>
+      </c>
+      <c r="N13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -956,37 +997,40 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.1366818755391422</v>
+        <v>-0.1667165938815502</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.1750142656652942</v>
+        <v>-0.237794433724694</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.1274747901520494</v>
+        <v>0.03548822600057738</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.1099795169164244</v>
+        <v>-0.01715540256640569</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5078689546094945</v>
+        <v>-1.54475956065185</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.3220252945300709</v>
+        <v>0.2250774747164198</v>
       </c>
       <c r="I14" t="n">
-        <v>0.06422451910516955</v>
+        <v>-0.07829168313764912</v>
       </c>
       <c r="J14" t="n">
-        <v>0.3893114657905196</v>
+        <v>0.06913708485703729</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.06198631201144565</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.7522081345985829</v>
+        <v>-0.3191331187553008</v>
       </c>
       <c r="M14" t="n">
-        <v>0.3398290965197098</v>
+        <v>-0.5377898646705344</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.260637167218768</v>
       </c>
     </row>
     <row r="15">
@@ -997,37 +1041,40 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.4054631955970956</v>
+        <v>-0.6017835588193785</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.1590029876281264</v>
+        <v>-0.2625286174864139</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1758221238658733</v>
+        <v>0.184392913661263</v>
       </c>
       <c r="F15" t="n">
-        <v>0.02945746199263036</v>
+        <v>-0.00298379784977932</v>
       </c>
       <c r="G15" t="n">
-        <v>0.8478342319935837</v>
+        <v>-1.198051117740401</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1637952423569879</v>
+        <v>0.4215129880059256</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.3714711427907169</v>
+        <v>-0.4167099952103409</v>
       </c>
       <c r="J15" t="n">
-        <v>0.7575482664842363</v>
+        <v>0.6122118655850348</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.084303640647092</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.879805721234389</v>
+        <v>-0.8356917463118756</v>
       </c>
       <c r="M15" t="n">
-        <v>1.118471141366099</v>
+        <v>-0.2932580846707885</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.8037272180612992</v>
       </c>
     </row>
     <row r="16">
@@ -1038,37 +1085,40 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.8151648081877648</v>
+        <v>-0.8083990037808713</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.3970624250334965</v>
+        <v>-0.585190120114677</v>
       </c>
       <c r="E16" t="n">
-        <v>1.593531493071227</v>
+        <v>1.255642220021523</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1304609186796717</v>
+        <v>0.1017024330965669</v>
       </c>
       <c r="G16" t="n">
-        <v>2.706367175311484</v>
+        <v>0.5077598605086806</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.1402338011813708</v>
+        <v>0.145546843617685</v>
       </c>
       <c r="I16" t="n">
-        <v>-3.089756073358634</v>
+        <v>-3.082730511717286</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1020274263008385</v>
+        <v>0.001178292720177221</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.1611525627603123</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>-1.425701416628885</v>
+        <v>0.02310003255828352</v>
       </c>
       <c r="M16" t="n">
-        <v>-1.130861331586144</v>
+        <v>-0.6973941088277145</v>
+      </c>
+      <c r="N16" t="n">
+        <v>-0.7978651073472509</v>
       </c>
     </row>
     <row r="17">
@@ -1079,37 +1129,40 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.6776215651655793</v>
+        <v>-0.7324020372522293</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.09601454979822999</v>
+        <v>-0.3357006862182667</v>
       </c>
       <c r="E17" t="n">
-        <v>1.600817869273732</v>
+        <v>1.139151097822506</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3064938536990633</v>
+        <v>0.3389023187740729</v>
       </c>
       <c r="G17" t="n">
-        <v>1.247092851018703</v>
+        <v>-0.6000760202575367</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.7766211674597</v>
+        <v>0.05046797699614627</v>
       </c>
       <c r="I17" t="n">
-        <v>-2.762626689935024</v>
+        <v>-2.944854497049232</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.0132398601477741</v>
+        <v>-0.01948303325890978</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.06128557859166428</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>-1.839844041346093</v>
+        <v>-0.9560737997243387</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.06307990344230563</v>
+        <v>-0.5504202117140521</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.604667271479058</v>
       </c>
     </row>
     <row r="18">
@@ -1120,37 +1173,40 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-2.244578921412165</v>
+        <v>-2.112431427998332</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.771860147026433</v>
+        <v>-0.1645494008336221</v>
       </c>
       <c r="E18" t="n">
-        <v>1.034253113333197</v>
+        <v>0.5695321672226028</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9708917912800484</v>
+        <v>0.468751069552042</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.695731686781095</v>
+        <v>-0.02292345180087502</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.150781054687765</v>
+        <v>-1.769032126737045</v>
       </c>
       <c r="I18" t="n">
-        <v>-5.668922668686251</v>
+        <v>-4.956724763580488</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.6185451931506004</v>
+        <v>-0.7663638356623007</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.7400711181697074</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>-2.334912970592486</v>
+        <v>-1.507056726530351</v>
       </c>
       <c r="M18" t="n">
-        <v>-2.614532489909299</v>
+        <v>2.319171186008474</v>
+      </c>
+      <c r="N18" t="n">
+        <v>-1.726398582041249</v>
       </c>
     </row>
     <row r="19">
@@ -1161,37 +1217,40 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.4271236777156054</v>
+        <v>-0.3635883797776742</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.2756839086638175</v>
+        <v>-0.02388291308980334</v>
       </c>
       <c r="E19" t="n">
-        <v>0.4173144834778058</v>
+        <v>0.1919618160697842</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1643044354897697</v>
+        <v>0.07461615955950603</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.3466460415028123</v>
+        <v>-0.003706049289695403</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.1894449594800967</v>
+        <v>-0.2853748882292213</v>
       </c>
       <c r="I19" t="n">
-        <v>-1.217952896645441</v>
+        <v>-0.9787222721180988</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.1070761385657463</v>
+        <v>-0.1259904405720858</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.1289650951224796</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.3276620759965734</v>
+        <v>-0.2068627853223666</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.5386458857125009</v>
+        <v>0.3786884658319962</v>
+      </c>
+      <c r="N19" t="n">
+        <v>-0.3174670141187252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the way balances works
</commit_message>
<xml_diff>
--- a/outputs/outperformance.xlsx
+++ b/outputs/outperformance.xlsx
@@ -461,40 +461,40 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.1489810950416438</v>
+        <v>-0.2594890654562015</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.2043474562481407</v>
+        <v>-0.2934520523824585</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.2547938095604285</v>
+        <v>-0.2494377539355348</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.0283171465889092</v>
+        <v>-0.03617483367244573</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.561687929733194</v>
+        <v>0.09003991013025806</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2521240374853275</v>
+        <v>0.1458347287376139</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.07928124633826795</v>
+        <v>-0.1399801602867078</v>
       </c>
       <c r="J2" t="n">
-        <v>0.02041826591931516</v>
+        <v>0.01939071256390057</v>
       </c>
       <c r="K2" t="n">
-        <v>0.02378011117973977</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.2098342518997854</v>
+        <v>-0.2926153968279041</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.5453174658749476</v>
+        <v>-0.05495139749410272</v>
       </c>
       <c r="N2" t="n">
-        <v>0.260637167218768</v>
+        <v>0.3388036330279748</v>
       </c>
     </row>
     <row r="3">
@@ -505,40 +505,40 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.4062303152217909</v>
+        <v>-0.4185302256558379</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.03086517683768375</v>
+        <v>-0.2234835412280841</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.2300319671529607</v>
+        <v>-0.2072920714574322</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.03032195891464575</v>
+        <v>-0.07166315892348649</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.186312698696654</v>
+        <v>0.2788672574637895</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3629622412102476</v>
+        <v>0.1973950443594833</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.5040763229969668</v>
+        <v>-0.7127793382414593</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6147778012059749</v>
+        <v>0.6341125469699391</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.2386391904336048</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>-2.109982518704936</v>
+        <v>-1.608942561718531</v>
       </c>
       <c r="M3" t="n">
-        <v>0.3768739117126277</v>
+        <v>0.7896345490914247</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8037272180612992</v>
+        <v>0.8703042820675433</v>
       </c>
     </row>
     <row r="4">
@@ -549,40 +549,40 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.7169975486779477</v>
+        <v>-1.22006804823917</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2946698798083034</v>
+        <v>0.010570696466361</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.06149789202139089</v>
+        <v>-2.050652521105039</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01091433704255712</v>
+        <v>0.1750662512221364</v>
       </c>
       <c r="G4" t="n">
-        <v>0.306022683792049</v>
+        <v>1.783504520762116</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1005380592722608</v>
+        <v>0.06828100991706487</v>
       </c>
       <c r="I4" t="n">
-        <v>-3.047512040033329</v>
+        <v>-1.090443284667019</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.1497267621519438</v>
+        <v>0.3246661265630818</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.02892383927239406</v>
+        <v>-0</v>
       </c>
       <c r="L4" t="n">
-        <v>-2.592559864161619</v>
+        <v>-1.001199160376046</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2672110784188562</v>
+        <v>0.7158355882672631</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.7978651073472509</v>
+        <v>-0.8639221881068608</v>
       </c>
     </row>
     <row r="5">
@@ -593,40 +593,40 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>-0.5414142807543174</v>
+        <v>-0.9789051338303025</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.007461755146021876</v>
+        <v>0.2832876626337821</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.08557828813120216</v>
+        <v>-2.140514980176671</v>
       </c>
       <c r="F5" t="n">
-        <v>0.274611466321977</v>
+        <v>0.411452656807904</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.7103281350806441</v>
+        <v>1.448833769525207</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.1362701662175447</v>
+        <v>-0.5686922471844291</v>
       </c>
       <c r="I5" t="n">
-        <v>-2.945418105643589</v>
+        <v>-1.256765309321006</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.08326532583783304</v>
+        <v>0.6025108545893475</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.2787265467134047</v>
+        <v>-0</v>
       </c>
       <c r="L5" t="n">
-        <v>-4.871307790857954</v>
+        <v>-1.746787450546593</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7994323085619569</v>
+        <v>1.301702462471367</v>
       </c>
       <c r="N5" t="n">
-        <v>0.604667271479058</v>
+        <v>-0.2285659650834222</v>
       </c>
     </row>
     <row r="6">
@@ -637,40 +637,40 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-1.273814175376051</v>
+        <v>-1.947080427264786</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8625605506452008</v>
+        <v>1.097773124942438</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3516343311900239</v>
+        <v>-2.678569806967828</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8295064829069797</v>
+        <v>1.482551069300036</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2646541652774737</v>
+        <v>2.134907188550496</v>
       </c>
       <c r="H6" t="n">
-        <v>-2.295526176009214</v>
+        <v>-1.548182035994453</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.359240583353815</v>
+        <v>-3.824684060090842</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.01152431248113572</v>
+        <v>0.8612236576940775</v>
       </c>
       <c r="K6" t="n">
-        <v>-1.349267970439772</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-10.56842778552956</v>
+        <v>-5.650182057401931</v>
       </c>
       <c r="M6" t="n">
-        <v>3.943185013355406</v>
+        <v>4.202965842269197</v>
       </c>
       <c r="N6" t="n">
-        <v>-1.726398582041249</v>
+        <v>-1.653149652953792</v>
       </c>
     </row>
     <row r="7">
@@ -681,40 +681,40 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.2142419044454809</v>
+        <v>-0.3444362924635327</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1503728058796788</v>
+        <v>0.1681585715117228</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.05601791128669487</v>
+        <v>-1.298318724003343</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1404504118786588</v>
+        <v>0.2359069376360411</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04807982169657055</v>
+        <v>0.3364880421999878</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.3776253217542895</v>
+        <v>-0.249257114077595</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.049080538168349</v>
+        <v>-0.6730524596865569</v>
       </c>
       <c r="J7" t="n">
-        <v>0.007488712061596708</v>
+        <v>0.1520416095900123</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.2382796914939904</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>-1.680918564179646</v>
+        <v>-0.919396568622477</v>
       </c>
       <c r="M7" t="n">
-        <v>0.6853788724589751</v>
+        <v>0.7230866621558039</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.3174670141187252</v>
+        <v>-0.3029257110927108</v>
       </c>
     </row>
     <row r="8">
@@ -729,37 +729,37 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.01773549883990645</v>
+        <v>0.03468264945443265</v>
       </c>
       <c r="D8" t="n">
-        <v>0.03344697747655328</v>
+        <v>0.02402384500745207</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.2902820355610058</v>
+        <v>-0.3495953757225437</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.01116174402250351</v>
+        <v>0.02183415705656238</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.01692836908134405</v>
+        <v>-0.006850299401198374</v>
       </c>
       <c r="H8" t="n">
-        <v>0.02704656276890775</v>
+        <v>0.004684701668394968</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.000989563200618839</v>
+        <v>-0.02011187388761828</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.04871881893772213</v>
+        <v>-0.0242115835286234</v>
       </c>
       <c r="K8" t="n">
-        <v>0.02378011117973977</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1092988668555154</v>
+        <v>-0.1063643457903465</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.007527601204413203</v>
+        <v>0.02699550074987656</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -773,37 +773,37 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.1955532435975876</v>
+        <v>0.2253262209110191</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2316634406487302</v>
+        <v>0.1136597030652758</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.4144248808142237</v>
+        <v>-0.4152909437775469</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.02733816106486643</v>
+        <v>0.02095401642685323</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01173841904374701</v>
+        <v>0.05446279599041853</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.05855074679567809</v>
+        <v>-0.04212149311311147</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.08736632778662594</v>
+        <v>-0.1534334619483862</v>
       </c>
       <c r="J9" t="n">
-        <v>0.002565935620940141</v>
+        <v>0.04028556482922666</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.2386391904336048</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>-1.274290772393061</v>
+        <v>-0.9621218509655438</v>
       </c>
       <c r="M9" t="n">
-        <v>0.6701319963834163</v>
+        <v>0.6915806363956095</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
@@ -817,37 +817,37 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.09140145510292352</v>
+        <v>0.1122520395495311</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2905202403063736</v>
+        <v>0.137652844838152</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.317140112042914</v>
+        <v>-1.644385879891446</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.09078809605400978</v>
+        <v>-0.06439117150823856</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.2017371767166316</v>
+        <v>-0.2772284572608367</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.04500878434542416</v>
+        <v>-0.03416341761919085</v>
       </c>
       <c r="I10" t="n">
-        <v>0.03521847168395729</v>
+        <v>0.03198665965268126</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.150905054872121</v>
+        <v>-0.1392669483330781</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.02892383927239406</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>-2.615659896719902</v>
+        <v>-1.788884105880865</v>
       </c>
       <c r="M10" t="n">
-        <v>0.9646051872465706</v>
+        <v>0.9954024011598053</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -861,37 +861,37 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1909877564979118</v>
+        <v>0.2389878252173965</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3282389310722448</v>
+        <v>0.1636148486915047</v>
       </c>
       <c r="E11" t="n">
-        <v>-1.224729385953708</v>
+        <v>-1.651636982109398</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.06429085245209593</v>
+        <v>-0.05078685021685899</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.1102521148231073</v>
+        <v>-0.1382479055080232</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.186738143213691</v>
+        <v>-0.1118639946266376</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.0005636085943564948</v>
+        <v>-0.02071681530078861</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.06378229257892326</v>
+        <v>-0.04300018881633662</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.2787265467134047</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>-3.915233991133615</v>
+        <v>-2.605765297647407</v>
       </c>
       <c r="M11" t="n">
-        <v>1.349852520276009</v>
+        <v>1.407403986358935</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -905,37 +905,37 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.8386172526222808</v>
+        <v>0.8990615323368752</v>
       </c>
       <c r="D12" t="n">
-        <v>1.027109951478823</v>
+        <v>0.4632329975338321</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.9211664984126267</v>
+        <v>-1.145093050071671</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3607554133549377</v>
+        <v>0.4245736807894576</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2875776170783487</v>
+        <v>0.4386466909671858</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.5264940492721689</v>
+        <v>-0.2937527160706956</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.4025158197733269</v>
+        <v>-0.5978546100523756</v>
       </c>
       <c r="J12" t="n">
-        <v>0.754839523181165</v>
+        <v>0.8805452787703727</v>
       </c>
       <c r="K12" t="n">
-        <v>-1.349267970439772</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>-9.061371058999205</v>
+        <v>-5.768774203058401</v>
       </c>
       <c r="M12" t="n">
-        <v>1.624013827346932</v>
+        <v>1.652283729358433</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -949,37 +949,37 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.1493464753321933</v>
+        <v>0.1596310907246765</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1742557189694822</v>
+        <v>0.07834268303374968</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.2479797273564791</v>
+        <v>-0.3051681095420896</v>
       </c>
       <c r="F13" t="n">
-        <v>0.06583425231915273</v>
+        <v>0.07691857335908939</v>
       </c>
       <c r="G13" t="n">
-        <v>0.05178587098626595</v>
+        <v>0.07862533823311679</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.0922504335250682</v>
+        <v>-0.05125319195938525</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.07035826605024999</v>
+        <v>-0.1040808282978039</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1334791526336825</v>
+        <v>0.1550415574641953</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.2382796914939904</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>-1.47405577885728</v>
+        <v>-0.9351569015473625</v>
       </c>
       <c r="M13" t="n">
-        <v>0.3066904066269789</v>
+        <v>0.3111619189530186</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -997,40 +997,40 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.1667165938815502</v>
+        <v>-0.2941717149106342</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.237794433724694</v>
+        <v>-0.3174758973899106</v>
       </c>
       <c r="E14" t="n">
-        <v>0.03548822600057738</v>
+        <v>0.1001576217870089</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.01715540256640569</v>
+        <v>-0.05800899072900811</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.54475956065185</v>
+        <v>0.09689020953145643</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2250774747164198</v>
+        <v>0.141150027069219</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.07829168313764912</v>
+        <v>-0.1198682863990895</v>
       </c>
       <c r="J14" t="n">
-        <v>0.06913708485703729</v>
+        <v>0.04360229609252397</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.3191331187553008</v>
+        <v>-0.1862510510375576</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.5377898646705344</v>
+        <v>-0.08194689824397927</v>
       </c>
       <c r="N14" t="n">
-        <v>0.260637167218768</v>
+        <v>0.3388036330279748</v>
       </c>
     </row>
     <row r="15">
@@ -1041,40 +1041,40 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.6017835588193785</v>
+        <v>-0.6438564465668569</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.2625286174864139</v>
+        <v>-0.3371432442933599</v>
       </c>
       <c r="E15" t="n">
-        <v>0.184392913661263</v>
+        <v>0.2079988723201147</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.00298379784977932</v>
+        <v>-0.09261717535033971</v>
       </c>
       <c r="G15" t="n">
-        <v>-1.198051117740401</v>
+        <v>0.224404461473371</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4215129880059256</v>
+        <v>0.2395165374725948</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.4167099952103409</v>
+        <v>-0.5593458762930731</v>
       </c>
       <c r="J15" t="n">
-        <v>0.6122118655850348</v>
+        <v>0.5938269821407125</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.8356917463118756</v>
+        <v>-0.6468207107529873</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.2932580846707885</v>
+        <v>0.0980539126958152</v>
       </c>
       <c r="N15" t="n">
-        <v>0.8037272180612992</v>
+        <v>0.8703042820675433</v>
       </c>
     </row>
     <row r="16">
@@ -1085,40 +1085,40 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.8083990037808713</v>
+        <v>-1.332320087788701</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.585190120114677</v>
+        <v>-0.127082148371791</v>
       </c>
       <c r="E16" t="n">
-        <v>1.255642220021523</v>
+        <v>-0.4062666412135938</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1017024330965669</v>
+        <v>0.239457422730375</v>
       </c>
       <c r="G16" t="n">
-        <v>0.5077598605086806</v>
+        <v>2.060732978022953</v>
       </c>
       <c r="H16" t="n">
-        <v>0.145546843617685</v>
+        <v>0.1024444275362557</v>
       </c>
       <c r="I16" t="n">
-        <v>-3.082730511717286</v>
+        <v>-1.1224299443197</v>
       </c>
       <c r="J16" t="n">
-        <v>0.001178292720177221</v>
+        <v>0.46393307489616</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="L16" t="n">
-        <v>0.02310003255828352</v>
+        <v>0.7876849455048192</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.6973941088277145</v>
+        <v>-0.2795668128925421</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.7978651073472509</v>
+        <v>-0.8639221881068608</v>
       </c>
     </row>
     <row r="17">
@@ -1129,40 +1129,40 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.7324020372522293</v>
+        <v>-1.217892959047699</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.3357006862182667</v>
+        <v>0.1196728139422774</v>
       </c>
       <c r="E17" t="n">
-        <v>1.139151097822506</v>
+        <v>-0.4888779980672731</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3389023187740729</v>
+        <v>0.462239507024763</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.6000760202575367</v>
+        <v>1.587081675033231</v>
       </c>
       <c r="H17" t="n">
-        <v>0.05046797699614627</v>
+        <v>-0.4568282525577915</v>
       </c>
       <c r="I17" t="n">
-        <v>-2.944854497049232</v>
+        <v>-1.236048494020218</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.01948303325890978</v>
+        <v>0.6455110434056841</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.9560737997243387</v>
+        <v>0.8589778471008143</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.5504202117140521</v>
+        <v>-0.105701523887568</v>
       </c>
       <c r="N17" t="n">
-        <v>0.604667271479058</v>
+        <v>-0.2285659650834222</v>
       </c>
     </row>
     <row r="18">
@@ -1173,40 +1173,40 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-2.112431427998332</v>
+        <v>-2.846141959601661</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.1645494008336221</v>
+        <v>0.6345401274086058</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5695321672226028</v>
+        <v>-1.533476756896157</v>
       </c>
       <c r="F18" t="n">
-        <v>0.468751069552042</v>
+        <v>1.057977388510578</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.02292345180087502</v>
+        <v>1.69626049758331</v>
       </c>
       <c r="H18" t="n">
-        <v>-1.769032126737045</v>
+        <v>-1.254429319923758</v>
       </c>
       <c r="I18" t="n">
-        <v>-4.956724763580488</v>
+        <v>-3.226829450038467</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.7663638356623007</v>
+        <v>-0.0193216210762952</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>-1.507056726530351</v>
+        <v>0.1185921456564696</v>
       </c>
       <c r="M18" t="n">
-        <v>2.319171186008474</v>
+        <v>2.550682112910764</v>
       </c>
       <c r="N18" t="n">
-        <v>-1.726398582041249</v>
+        <v>-1.653149652953792</v>
       </c>
     </row>
     <row r="19">
@@ -1217,40 +1217,40 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.3635883797776742</v>
+        <v>-0.5040673831882092</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.02388291308980334</v>
+        <v>0.08981588847797307</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1919618160697842</v>
+        <v>-0.9931506144612535</v>
       </c>
       <c r="F19" t="n">
-        <v>0.07461615955950603</v>
+        <v>0.1589883642769518</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.003706049289695403</v>
+        <v>0.2578627039668711</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.2853748882292213</v>
+        <v>-0.1980039221182097</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.9787222721180988</v>
+        <v>-0.568971631388753</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.1259904405720858</v>
+        <v>-0.002999947874183007</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.2068627853223666</v>
+        <v>0.01576033292488555</v>
       </c>
       <c r="M19" t="n">
-        <v>0.3786884658319962</v>
+        <v>0.4119247432027853</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.3174670141187252</v>
+        <v>-0.3029257110927108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>